<commit_message>
fix: fix column header in clopidogrel test alert file
</commit_message>
<xml_diff>
--- a/clopidogrel/Clopidogrel_Pre_and_Post_Test_Alerts.xlsx
+++ b/clopidogrel/Clopidogrel_Pre_and_Post_Test_Alerts.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11010"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MCPHS Faculty\CPIC Job\CYP2C19_clopidogrel update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katrin/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9C6B66E-0691-4C53-88F4-C525FEB23801}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E19946F3-C7E9-B948-9E26-BEBD68BE5DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="24440" windowHeight="15000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="population general" sheetId="1" r:id="rId1"/>
-    <sheet name="Flow Chart" sheetId="3" r:id="rId2"/>
-    <sheet name="Change log" sheetId="4" r:id="rId3"/>
+    <sheet name="Change log" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,9 +44,6 @@
   </si>
   <si>
     <t>Post-Test</t>
-  </si>
-  <si>
-    <t>Activity Score</t>
   </si>
   <si>
     <t>n/a</t>
@@ -190,6 +186,9 @@
   </si>
   <si>
     <t>Based on the genotype result, this patient is predicted to be a CYP2C19 poor metabolizer. Avoid clopidogrel if possible due to the risk of therapeutic failure. Use an alternative antiplatelet agent at standard dose if no contraindication. Prasugrel is contraindicated in patients with a history of transient ischemic attack or stroke. Please consult a clinical pharmacist for more information.</t>
+  </si>
+  <si>
+    <t>CYP2C19 Activity Score</t>
   </si>
 </sst>
 </file>
@@ -320,55 +319,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>103771</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>18605</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{874CA8A1-8B3D-433F-84EC-798B93CF8398}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="8028571" cy="3561905"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -636,218 +586,216 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.58203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="8.08203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="19.58203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="103.25" style="2" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="103.1640625" style="2" customWidth="1"/>
     <col min="6" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>10</v>
-      </c>
       <c r="C1" s="13" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="31" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="31" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>14</v>
-      </c>
       <c r="C5" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="62" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>21</v>
-      </c>
       <c r="C8" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="68" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>2</v>
       </c>
       <c r="E9" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="8"/>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
     </row>
-    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -861,40 +809,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{137D04FA-ECB8-4896-B7D9-173CD77BC6BD}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>24</v>
       </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="14">
         <v>44411</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>